<commit_message>
error tocho en rings
procedo a hacer cambios tochos a esto
</commit_message>
<xml_diff>
--- a/data/Kanaleneiland/archetypes/pop_archetypes_citizen.xlsx
+++ b/data/Kanaleneiland/archetypes/pop_archetypes_citizen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\data\Kanaleneiland\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975E3EF0-8D04-4E87-BC3F-8C70D2E84F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252A6E63-24A2-4A4D-8CE8-F2319B9C6FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="855" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,10 +747,10 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AE2">
-        <v>9.4499999999999993</v>
+        <v>9.4529999999999994</v>
       </c>
       <c r="AF2">
-        <v>9.1999999999999998E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="AG2">
         <v>9.5839999999999996</v>
@@ -851,10 +851,10 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="AE3">
-        <v>9.2439999999999998</v>
+        <v>9.2490000000000006</v>
       </c>
       <c r="AF3">
-        <v>0.122</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="AG3">
         <v>9.2739999999999991</v>
@@ -955,10 +955,10 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="AE4">
-        <v>7.569</v>
+        <v>8.2430000000000003</v>
       </c>
       <c r="AF4">
-        <v>0.217</v>
+        <v>0.105</v>
       </c>
       <c r="AG4">
         <v>8.8160000000000007</v>
@@ -1059,10 +1059,10 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="AE5">
-        <v>8.5990000000000002</v>
+        <v>8.66</v>
       </c>
       <c r="AF5">
-        <v>0.40899999999999997</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="AG5">
         <v>9.2690000000000001</v>
@@ -1163,10 +1163,10 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="AE6">
-        <v>9.1579999999999995</v>
+        <v>9.4120000000000008</v>
       </c>
       <c r="AF6">
-        <v>0.19500000000000001</v>
+        <v>0.105</v>
       </c>
       <c r="AG6">
         <v>9.5090000000000003</v>

</xml_diff>